<commit_message>
Social competence feature generation. Utilities: drawing a sample from a distribution, converting a list of dicts to a dict of lists (to create a dataframe from them)
</commit_message>
<xml_diff>
--- a/data/processed/poland/DW/age_gender.xlsx
+++ b/data/processed/poland/DW/age_gender.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="processed" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="processed_old" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="raw" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="processed" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t xml:space="preserve">Age</t>
   </si>
@@ -234,6 +235,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -394,8 +396,8 @@
   </sheetPr>
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2650,7 +2652,636 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>7215</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>3698</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>3517</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>7474</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>3821</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>7319</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>3748</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>6974</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>3596</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>3378</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>6663</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>3469</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>3194</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>6459</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>3389</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>6193</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>3217</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>2976</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>6266</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>3239</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>6384</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>3292</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>6383</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>3268</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>3115</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>6242</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>3160</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>5762</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>2904</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>2858</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>5312</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>2716</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>4928</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>2526</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>2402</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>4494</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>2299</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>4244</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>2152</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>4206</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>2099</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>4419</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>2199</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>4503</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>2255</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>4630</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>2336</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>4896</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>2507</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>5057</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>2613</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>5168</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>2619</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>2549</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>5133</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>2617</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>5418</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>2750</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>5857</v>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>2909</v>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>2948</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>5881</v>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>2934</v>
+      </c>
+      <c r="D28" s="4" t="n">
+        <v>2947</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>7064</v>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>3403</v>
+      </c>
+      <c r="D29" s="4" t="n">
+        <v>3661</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="n">
+        <v>8920</v>
+      </c>
+      <c r="C30" s="4" t="n">
+        <v>4192</v>
+      </c>
+      <c r="D30" s="4" t="n">
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>9860</v>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>4662</v>
+      </c>
+      <c r="D31" s="4" t="n">
+        <v>5198</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>61821</v>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>29436</v>
+      </c>
+      <c r="D32" s="4" t="n">
+        <v>32385</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>65283</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>32352</v>
+      </c>
+      <c r="D33" s="4" t="n">
+        <v>32931</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>52762</v>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>26055</v>
+      </c>
+      <c r="D34" s="4" t="n">
+        <v>26707</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>39349</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>19507</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <v>19842</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>31693</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>15332</v>
+      </c>
+      <c r="D36" s="4" t="n">
+        <v>16361</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>34595</v>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>15893</v>
+      </c>
+      <c r="D37" s="4" t="n">
+        <v>18702</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>45638</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <v>20333</v>
+      </c>
+      <c r="D38" s="4" t="n">
+        <v>25305</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>45373</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>19180</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <v>26193</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>31279</v>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>12749</v>
+      </c>
+      <c r="D40" s="4" t="n">
+        <v>18530</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>18952</v>
+      </c>
+      <c r="C41" s="4" t="n">
+        <v>7037</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <v>11915</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="4" t="n">
+        <v>17194</v>
+      </c>
+      <c r="C42" s="4" t="n">
+        <v>5838</v>
+      </c>
+      <c r="D42" s="4" t="n">
+        <v>11356</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <v>18344</v>
+      </c>
+      <c r="C43" s="4" t="n">
+        <v>5352</v>
+      </c>
+      <c r="D43" s="4" t="n">
+        <v>12992</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>